<commit_message>
updated the Auswertung.xlsx file
</commit_message>
<xml_diff>
--- a/evaluation images/Auswertung.xlsx
+++ b/evaluation images/Auswertung.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23540" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Frameworks" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="69">
   <si>
     <t>Vision</t>
   </si>
@@ -228,6 +228,9 @@
   <si>
     <t>Wertung</t>
   </si>
+  <si>
+    <t>Unbekannte Eigenentwicklung</t>
+  </si>
 </sst>
 </file>
 
@@ -302,8 +305,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="977">
+  <cellStyleXfs count="993">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1329,7 +1348,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="977">
+  <cellStyles count="993">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1818,6 +1837,14 @@
     <cellStyle name="Followed Hyperlink" xfId="972" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="974" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="976" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="978" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="980" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="982" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="984" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="986" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="988" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="990" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="992" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2306,6 +2333,14 @@
     <cellStyle name="Hyperlink" xfId="971" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="973" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="975" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="977" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="979" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="981" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="983" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="985" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="987" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="989" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="991" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2349,9 +2384,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Frameworks!$A$1:$A$9</c:f>
+              <c:f>Frameworks!$A$1:$A$10</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Scanner SDK</c:v>
                 </c:pt>
@@ -2368,15 +2403,18 @@
                   <c:v>Genius Scan SDK</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>Unbekannte Eigenentwicklung</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>OpenCV</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>GPUImage</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Vision</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>GPUImage</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>CIDetector</c:v>
                 </c:pt>
               </c:strCache>
@@ -2384,10 +2422,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Frameworks!$B$1:$B$9</c:f>
+              <c:f>Frameworks!$B$1:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -2410,10 +2448,13 @@
                   <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17.0</c:v>
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3952,6 +3993,9 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>0.4172</c:v>
                 </c:pt>
@@ -4321,10 +4365,10 @@
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>558800</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4928,15 +4972,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S41" sqref="S41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -4981,7 +5025,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>68</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -4989,7 +5033,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -5000,19 +5044,28 @@
         <v>0</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
         <v>1</v>
       </c>
-      <c r="B9">
-        <v>17</v>
+      <c r="B10">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -5244,8 +5297,8 @@
   <dimension ref="A1:I231"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G61" sqref="G61"/>
+      <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F164" sqref="F164:F171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8315,9 +8368,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I231"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A204" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G235" sqref="G235"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A156" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B165" sqref="B165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11020,7 +11073,9 @@
       <c r="E224" t="s">
         <v>63</v>
       </c>
-      <c r="F224" s="10"/>
+      <c r="F224" s="10">
+        <v>0</v>
+      </c>
       <c r="G224" s="10">
         <f>1-F224</f>
         <v>1</v>

</xml_diff>